<commit_message>
updated code and sample excel
</commit_message>
<xml_diff>
--- a/gend sample.xlsx
+++ b/gend sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Others\StreamLit_Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB921BA4-3055-4BB6-A7C8-AF24AD1A6C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96B8143-D721-4E5C-936E-F9641F49054B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" xr2:uid="{F00BC979-6386-4C2B-AEF5-4AAF9356E276}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>Maria John</t>
+  </si>
+  <si>
+    <t>Justine Faith</t>
+  </si>
+  <si>
+    <t>Timothy Jonah</t>
+  </si>
+  <si>
+    <t>Justin John</t>
   </si>
 </sst>
 </file>
@@ -427,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{292BC4E9-0B32-48A9-861E-C4C006E71094}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -501,6 +510,21 @@
         <v>13</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>